<commit_message>
Added Error Percentage Calculation Look at the bottem line in the execel file
</commit_message>
<xml_diff>
--- a/Heavy Rain.xlsx
+++ b/Heavy Rain.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="144" windowWidth="22980" windowHeight="8760" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="150" windowWidth="20610" windowHeight="8760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="4" r:id="rId1"/>
@@ -4689,11 +4689,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="215378560"/>
-        <c:axId val="215384448"/>
+        <c:axId val="138324224"/>
+        <c:axId val="138334208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="215378560"/>
+        <c:axId val="138324224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4702,7 +4702,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="215384448"/>
+        <c:crossAx val="138334208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4710,7 +4710,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="215384448"/>
+        <c:axId val="138334208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4721,14 +4721,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="215378560"/>
+        <c:crossAx val="138324224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8420,11 +8419,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="127035648"/>
-        <c:axId val="127037440"/>
+        <c:axId val="146065664"/>
+        <c:axId val="146067456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="127035648"/>
+        <c:axId val="146065664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8433,7 +8432,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127037440"/>
+        <c:crossAx val="146067456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8441,7 +8440,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="127037440"/>
+        <c:axId val="146067456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8452,14 +8451,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127035648"/>
+        <c:crossAx val="146065664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8834,13 +8832,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F268" activeCellId="3" sqref="I1:I1048576 H1:H1048576 G1:G1048576 F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8869,7 +8867,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>146.16669999999999</v>
       </c>
@@ -8898,7 +8896,7 @@
         <v>146.16669999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>131.55002999999999</v>
       </c>
@@ -8927,7 +8925,7 @@
         <v>14.616669999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>118.395027</v>
       </c>
@@ -8956,7 +8954,7 @@
         <v>1.461667</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>106.5555243</v>
       </c>
@@ -8985,7 +8983,7 @@
         <v>0.14616670000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>124.69997187</v>
       </c>
@@ -9014,7 +9012,7 @@
         <v>259.21461667</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>112.22997468299999</v>
       </c>
@@ -9043,7 +9041,7 @@
         <v>25.921461666999999</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>110.906977215</v>
       </c>
@@ -9072,7 +9070,7 @@
         <v>91.692146166699999</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>99.8162794932</v>
       </c>
@@ -9101,7 +9099,7 @@
         <v>9.1692146166700006</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>95.834651543899994</v>
       </c>
@@ -9130,7 +9128,7 @@
         <v>54.916921461699999</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>87.151186389499998</v>
       </c>
@@ -9159,7 +9157,7 @@
         <v>13.5916921462</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>79.936067750600003</v>
       </c>
@@ -9188,7 +9186,7 @@
         <v>14.8591692146</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>72.242460975499995</v>
       </c>
@@ -9217,7 +9215,7 @@
         <v>4.1859169214599996</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>65.018214877999995</v>
       </c>
@@ -9246,7 +9244,7 @@
         <v>0.41859169214600001</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>65.4163933902</v>
       </c>
@@ -9275,7 +9273,7 @@
         <v>62.141859169200004</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>64.274754051100004</v>
       </c>
@@ -9304,7 +9302,7 @@
         <v>54.814185916900001</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>64.447278646000001</v>
       </c>
@@ -9333,7 +9331,7 @@
         <v>64.881418591699997</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>68.502550781400004</v>
       </c>
@@ -9362,7 +9360,7 @@
         <v>100.988141859</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>69.627295703300007</v>
       </c>
@@ -9391,7 +9389,7 @@
         <v>81.873814185900002</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>62.664566133000001</v>
       </c>
@@ -9420,7 +9418,7 @@
         <v>8.1873814185900002</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>62.098109519700003</v>
       </c>
@@ -9449,7 +9447,7 @@
         <v>52.118738141900003</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>55.888298567699998</v>
       </c>
@@ -9478,7 +9476,7 @@
         <v>5.2118738141899996</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>50.299468710900001</v>
       </c>
@@ -9507,7 +9505,7 @@
         <v>0.52118738141900001</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>76.169521839799998</v>
       </c>
@@ -9536,7 +9534,7 @@
         <v>278.15211873800001</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>68.552569655799999</v>
       </c>
@@ -9565,7 +9563,7 @@
         <v>27.815211873799999</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>61.697312690300002</v>
       </c>
@@ -9594,7 +9592,7 @@
         <v>2.7815211873800001</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>83.127581421200006</v>
       </c>
@@ -9623,7 +9621,7 @@
         <v>248.678152119</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>74.814823279099997</v>
       </c>
@@ -9652,7 +9650,7 @@
         <v>24.867815211900002</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>67.3333409512</v>
       </c>
@@ -9681,7 +9679,7 @@
         <v>2.4867815211900002</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>64.200006856100003</v>
       </c>
@@ -9710,7 +9708,7 @@
         <v>32.648678152099997</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>57.780006170500002</v>
       </c>
@@ -9739,7 +9737,7 @@
         <v>3.2648678152100001</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>52.002005553399997</v>
       </c>
@@ -9768,7 +9766,7 @@
         <v>0.32648678152100002</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>46.801804998100003</v>
       </c>
@@ -9797,7 +9795,7 @@
         <v>3.26486781521E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>46.0216244983</v>
       </c>
@@ -9826,7 +9824,7 @@
         <v>35.1032648678</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>48.9194620484</v>
       </c>
@@ -9855,7 +9853,7 @@
         <v>71.010326486799997</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>45.227515843600003</v>
       </c>
@@ -9884,7 +9882,7 @@
         <v>17.901032648699999</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>40.704764259199997</v>
       </c>
@@ -9913,7 +9911,7 @@
         <v>1.7901032648699999</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>54.6342878333</v>
       </c>
@@ -9942,7 +9940,7 @@
         <v>162.179010326</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>76.470859050000001</v>
       </c>
@@ -9971,7 +9969,7 @@
         <v>261.91790103300002</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>88.623773145000001</v>
       </c>
@@ -10000,7 +9998,7 @@
         <v>204.39179010300001</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>82.161395830499998</v>
       </c>
@@ -10029,7 +10027,7 @@
         <v>42.039179010300003</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>73.945256247399996</v>
       </c>
@@ -10058,7 +10056,7 @@
         <v>4.2039179010299996</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>74.950730622699993</v>
       </c>
@@ -10087,7 +10085,7 @@
         <v>76.020391790100007</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>67.455657560399999</v>
       </c>
@@ -10116,7 +10114,7 @@
         <v>7.6020391790100001</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>61.6100918044</v>
       </c>
@@ -10145,7 +10143,7 @@
         <v>8.8602039178999998</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>77.349082623900003</v>
       </c>
@@ -10174,7 +10172,7 @@
         <v>197.986020392</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>77.314174361599996</v>
       </c>
@@ -10203,7 +10201,7 @@
         <v>89.098602039200003</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>69.582756925400005</v>
       </c>
@@ -10232,7 +10230,7 @@
         <v>8.9098602039199992</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>62.624481232900003</v>
       </c>
@@ -10261,7 +10259,7 @@
         <v>0.89098602039200003</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>64.162033109600003</v>
       </c>
@@ -10290,7 +10288,7 @@
         <v>70.289098601999996</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>78.712499798600007</v>
       </c>
@@ -10319,7 +10317,7 @@
         <v>195.72893986</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>79.841249818799994</v>
       </c>
@@ -10348,7 +10346,7 @@
         <v>100.572893986</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>79.057124836900002</v>
       </c>
@@ -10377,7 +10375,7 @@
         <v>74.857289398600003</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>72.051412353200007</v>
       </c>
@@ -10406,7 +10404,7 @@
         <v>15.585728939899999</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>64.846271117900002</v>
       </c>
@@ -10435,7 +10433,7 @@
         <v>1.5585728939900001</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>58.361644006100001</v>
       </c>
@@ -10464,7 +10462,7 @@
         <v>0.15585728939900001</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56.725479605499999</v>
       </c>
@@ -10493,7 +10491,7 @@
         <v>37.815585728899997</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>60.952931644899998</v>
       </c>
@@ -10522,7 +10520,7 @@
         <v>92.881558572900005</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>56.357638480399999</v>
       </c>
@@ -10551,7 +10549,7 @@
         <v>22.788155857300001</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>52.521874632399999</v>
       </c>
@@ -10580,7 +10578,7 @@
         <v>18.478815585700001</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>61.369687169199999</v>
       </c>
@@ -10609,7 +10607,7 @@
         <v>128.74788155900001</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60.032718452200001</v>
       </c>
@@ -10638,7 +10636,7 @@
         <v>56.074788155900002</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>56.729446607</v>
       </c>
@@ -10667,7 +10665,7 @@
         <v>29.907478815600001</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>51.056501946300003</v>
       </c>
@@ -10696,7 +10694,7 @@
         <v>2.9907478815599999</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>49.850851751699999</v>
       </c>
@@ -10725,7 +10723,7 @@
         <v>35.399074788199997</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>48.165766576499998</v>
       </c>
@@ -10754,7 +10752,7 @@
         <v>33.239907478799999</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>43.349189918900002</v>
       </c>
@@ -10783,7 +10781,7 @@
         <v>3.3239907478799999</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>39.014270926999998</v>
       </c>
@@ -10812,7 +10810,7 @@
         <v>0.33239907478800002</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>36.0128438343</v>
       </c>
@@ -10841,7 +10839,7 @@
         <v>8.1332399074800001</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>40.211559450800003</v>
       </c>
@@ -10870,7 +10868,7 @@
         <v>71.013323990700002</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>36.190403505799999</v>
       </c>
@@ -10899,7 +10897,7 @@
         <v>7.1013323990700004</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>32.571363155199997</v>
       </c>
@@ -10928,7 +10926,7 @@
         <v>0.71013323990699995</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>36.814226839699998</v>
       </c>
@@ -10957,7 +10955,7 @@
         <v>67.571013324000006</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>37.632804155700001</v>
       </c>
@@ -10986,7 +10984,7 @@
         <v>47.257101332399998</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>49.769523740099999</v>
       </c>
@@ -11015,7 +11013,7 @@
         <v>147.825710133</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>46.592571366100003</v>
       </c>
@@ -11044,7 +11042,7 @@
         <v>30.982571013299999</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>47.933314229499999</v>
       </c>
@@ -11073,7 +11071,7 @@
         <v>57.0982571013</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>44.039982806600001</v>
       </c>
@@ -11102,7 +11100,7 @@
         <v>13.8098257101</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>64.535984525900005</v>
       </c>
@@ -11131,7 +11129,7 @@
         <v>225.480982571</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>81.182386073299995</v>
       </c>
@@ -11160,7 +11158,7 @@
         <v>230.448098257</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>102.822487466</v>
       </c>
@@ -11189,7 +11187,7 @@
         <v>290.86986982600001</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>99.740238719399997</v>
       </c>
@@ -11218,7 +11216,7 @@
         <v>93.886986982600007</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>91.766214847399993</v>
       </c>
@@ -11247,7 +11245,7 @@
         <v>27.388698698300001</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>82.589593362700001</v>
       </c>
@@ -11276,7 +11274,7 @@
         <v>2.7388698698299998</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>74.330634026400006</v>
       </c>
@@ -11305,7 +11303,7 @@
         <v>0.27388698698300001</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>66.897570623799993</v>
       </c>
@@ -11334,7 +11332,7 @@
         <v>2.7388698698300001E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>60.207813561400002</v>
       </c>
@@ -11363,7 +11361,7 @@
         <v>2.7388698698299998E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>54.1870322053</v>
       </c>
@@ -11392,7 +11390,7 @@
         <v>2.7388698698299998E-4</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>53.568328984700003</v>
       </c>
@@ -11421,7 +11419,7 @@
         <v>43.200027388700001</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>51.611496086300001</v>
       </c>
@@ -11450,7 +11448,7 @@
         <v>34.920002738900003</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>46.4503464776</v>
       </c>
@@ -11479,7 +11477,7 @@
         <v>3.49200027389</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>50.205311829899998</v>
       </c>
@@ -11508,7 +11506,7 @@
         <v>75.949200027399996</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>45.184780646900002</v>
       </c>
@@ -11537,7 +11535,7 @@
         <v>7.5949200027400003</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>40.666302582199997</v>
       </c>
@@ -11566,7 +11564,7 @@
         <v>0.75949200027399999</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>49.599672323999997</v>
       </c>
@@ -11595,7 +11593,7 @@
         <v>117.0759492</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>44.6397050916</v>
       </c>
@@ -11624,7 +11622,7 @@
         <v>11.70759492</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>40.475734582400001</v>
       </c>
@@ -11653,7 +11651,7 @@
         <v>3.8707594919999999</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>36.428161124200003</v>
       </c>
@@ -11682,7 +11680,7 @@
         <v>0.38707594919999999</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>32.785345011799997</v>
       </c>
@@ -11711,7 +11709,7 @@
         <v>3.8707594919999998E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>29.506810510600001</v>
       </c>
@@ -11740,7 +11738,7 @@
         <v>3.8707594919999999E-3</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>26.556129459499999</v>
       </c>
@@ -11769,7 +11767,7 @@
         <v>3.8707594919999998E-4</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>24.800516513600002</v>
       </c>
@@ -11798,7 +11796,7 @@
         <v>8.1000387075900004</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>22.620464862199999</v>
       </c>
@@ -11827,7 +11825,7 @@
         <v>3.5100038707599999</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>25.758418376000002</v>
       </c>
@@ -11856,7 +11854,7 @@
         <v>48.951000387100002</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>24.682576538399999</v>
       </c>
@@ -11885,7 +11883,7 @@
         <v>18.395100038700001</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>25.614318884599999</v>
       </c>
@@ -11914,7 +11912,7 @@
         <v>32.439510003899997</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>23.0528869961</v>
       </c>
@@ -11943,7 +11941,7 @@
         <v>3.2439510003900001</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>20.747598296500001</v>
       </c>
@@ -11972,7 +11970,7 @@
         <v>0.32439510003900002</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>29.172838466799998</v>
       </c>
@@ -12001,7 +11999,7 @@
         <v>94.532439510000003</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>42.455554620199997</v>
       </c>
@@ -12030,7 +12028,7 @@
         <v>155.253243951</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>45.109999158100003</v>
       </c>
@@ -12059,7 +12057,7 @@
         <v>77.625324395099994</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>67.298999242299999</v>
       </c>
@@ -12088,7 +12086,7 @@
         <v>248.06253244000001</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>64.469099318100007</v>
       </c>
@@ -12117,7 +12115,7 @@
         <v>59.906253243999998</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>67.022189386299999</v>
       </c>
@@ -12146,7 +12144,7 @@
         <v>86.9906253244</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>78.019970447700004</v>
       </c>
@@ -12175,7 +12173,7 @@
         <v>167.99906253200001</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>70.2179734029</v>
       </c>
@@ -12204,7 +12202,7 @@
         <v>16.7999062532</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>66.4961760626</v>
       </c>
@@ -12233,7 +12231,7 @@
         <v>31.3799906253</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>59.846558456300002</v>
       </c>
@@ -12262,7 +12260,7 @@
         <v>3.13799906253</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>53.8619026107</v>
       </c>
@@ -12291,7 +12289,7 @@
         <v>0.31379990625300003</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>51.475712349600002</v>
       </c>
@@ -12320,7 +12318,7 @@
         <v>27.031379990600001</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>46.6281411147</v>
       </c>
@@ -12349,7 +12347,7 @@
         <v>5.4031379990600001</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>41.965327003200002</v>
       </c>
@@ -12378,7 +12376,7 @@
         <v>0.54031379990600004</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>37.768794302899998</v>
       </c>
@@ -12407,7 +12405,7 @@
         <v>5.4031379990600002E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>33.991914872599999</v>
       </c>
@@ -12436,7 +12434,7 @@
         <v>5.4031379990600002E-3</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>30.892723385299998</v>
       </c>
@@ -12465,7 +12463,7 @@
         <v>2.7005403137999999</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>27.803451046799999</v>
       </c>
@@ -12494,7 +12492,7 @@
         <v>0.27005403138</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>25.023105942099999</v>
       </c>
@@ -12523,7 +12521,7 @@
         <v>2.7005403138000001E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>22.520795347899998</v>
       </c>
@@ -12552,7 +12550,7 @@
         <v>2.7005403137999998E-3</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>20.268715813099998</v>
       </c>
@@ -12581,7 +12579,7 @@
         <v>2.7005403137999998E-4</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>27.541844231799999</v>
       </c>
@@ -12610,7 +12608,7 @@
         <v>83.700027005400003</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>24.787659808600001</v>
       </c>
@@ -12639,7 +12637,7 @@
         <v>8.3700027005400006</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>22.308893827799999</v>
       </c>
@@ -12668,7 +12666,7 @@
         <v>0.83700027005400002</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>20.078004445000001</v>
       </c>
@@ -12697,7 +12695,7 @@
         <v>8.3700027005399996E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>79.270204000500001</v>
       </c>
@@ -12726,7 +12724,7 @@
         <v>550.80837000300005</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>82.143183600399993</v>
       </c>
@@ -12755,7 +12753,7 @@
         <v>152.28083699999999</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>73.9288652404</v>
       </c>
@@ -12784,7 +12782,7 @@
         <v>15.228083699999999</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>68.335978716400007</v>
       </c>
@@ -12813,7 +12811,7 @@
         <v>17.722808369999999</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>90.302380844699996</v>
       </c>
@@ -12842,7 +12840,7 @@
         <v>260.97228083700003</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>87.772142760199998</v>
       </c>
@@ -12871,7 +12869,7 @@
         <v>84.597228083700003</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>78.994928484200003</v>
       </c>
@@ -12900,7 +12898,7 @@
         <v>8.4597228083699996</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>71.095435635800001</v>
       </c>
@@ -12929,7 +12927,7 @@
         <v>0.84597228083700005</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>63.985892072200002</v>
       </c>
@@ -12958,7 +12956,7 @@
         <v>8.4597228083700002E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>57.587302864999998</v>
       </c>
@@ -12987,7 +12985,7 @@
         <v>8.4597228083700005E-3</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>76.128572578499998</v>
       </c>
@@ -13016,7 +13014,7 @@
         <v>218.700845972</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>68.515715320599995</v>
       </c>
@@ -13045,7 +13043,7 @@
         <v>21.870084597200002</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>64.064143788600006</v>
       </c>
@@ -13074,7 +13072,7 @@
         <v>23.787008459700001</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>57.657729409700003</v>
       </c>
@@ -13103,7 +13101,7 @@
         <v>2.3787008459700001</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>51.891956468799997</v>
       </c>
@@ -13132,7 +13130,7 @@
         <v>0.23787008459699999</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>52.7027608219</v>
       </c>
@@ -13161,7 +13159,7 @@
         <v>54.023787008500001</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>53.132484739699997</v>
       </c>
@@ -13190,7 +13188,7 @@
         <v>56.702378700799997</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>53.819236265699999</v>
       </c>
@@ -13219,7 +13217,7 @@
         <v>59.670237870100003</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>48.4373126391</v>
       </c>
@@ -13248,7 +13246,7 @@
         <v>5.9670237870099996</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>51.093581375200003</v>
       </c>
@@ -13277,7 +13275,7 @@
         <v>68.096702378700002</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>76.284223237700004</v>
       </c>
@@ -13306,7 +13304,7 @@
         <v>279.50967023800001</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>93.255800913900003</v>
       </c>
@@ -13335,7 +13333,7 @@
         <v>249.350967024</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>89.330220822499996</v>
       </c>
@@ -13364,7 +13362,7 @@
         <v>73.535096702399997</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>86.997198740300007</v>
       </c>
@@ -13393,7 +13391,7 @@
         <v>66.753509670200003</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>78.297478866299997</v>
       </c>
@@ -13422,7 +13420,7 @@
         <v>6.67535096702</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>74.667730979599995</v>
       </c>
@@ -13451,7 +13449,7 @@
         <v>38.467535096699997</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>69.000957881700003</v>
       </c>
@@ -13480,7 +13478,7 @@
         <v>20.0467535097</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>63.500862093499997</v>
       </c>
@@ -13509,7 +13507,7 @@
         <v>14.604675350999999</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>64.950775884199999</v>
       </c>
@@ -13538,7 +13536,7 @@
         <v>71.660467535099997</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>64.155698295700006</v>
       </c>
@@ -13567,7 +13565,7 @@
         <v>58.466046753500002</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>75.140128466199997</v>
       </c>
@@ -13596,7 +13594,7 @@
         <v>162.446604675</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>84.126115619499998</v>
       </c>
@@ -13625,7 +13623,7 @@
         <v>164.74466046800001</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>82.613504057599997</v>
       </c>
@@ -13654,7 +13652,7 @@
         <v>78.574466046799998</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>94.7521536518</v>
       </c>
@@ -13683,7 +13681,7 @@
         <v>191.457446605</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>93.976938286700005</v>
       </c>
@@ -13712,7 +13710,7 @@
         <v>97.445744660499997</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>90.279244457999994</v>
       </c>
@@ -13741,7 +13739,7 @@
         <v>61.044574466</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>91.151320012200003</v>
       </c>
@@ -13770,7 +13768,7 @@
         <v>95.204457446600003</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>83.236188010999996</v>
       </c>
@@ -13799,7 +13797,7 @@
         <v>20.320445744699999</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>75.212569209899996</v>
       </c>
@@ -13828,7 +13826,7 @@
         <v>4.7320445744699997</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>97.091312288899999</v>
       </c>
@@ -13857,7 +13855,7 @@
         <v>265.07320445699997</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>93.082181059999996</v>
       </c>
@@ -13886,7 +13884,7 @@
         <v>77.8073204457</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>83.773962953999998</v>
       </c>
@@ -13915,7 +13913,7 @@
         <v>7.7807320445699997</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>75.396566658599994</v>
       </c>
@@ -13944,7 +13942,7 @@
         <v>0.77807320445700001</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>74.156909992699994</v>
       </c>
@@ -13973,7 +13971,7 @@
         <v>56.777807320400001</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>94.041218993499996</v>
       </c>
@@ -14002,7 +14000,7 @@
         <v>251.37778073199999</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>88.537097094100005</v>
       </c>
@@ -14031,7 +14029,7 @@
         <v>60.237778073199998</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>79.683387384699998</v>
       </c>
@@ -14060,7 +14058,7 @@
         <v>6.0237778073200001</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>71.715048646200003</v>
       </c>
@@ -14089,7 +14087,7 @@
         <v>0.60237778073199999</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>64.543543781599993</v>
       </c>
@@ -14118,7 +14116,7 @@
         <v>6.02377780732E-2</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>58.089189403500001</v>
       </c>
@@ -14147,7 +14145,7 @@
         <v>6.02377780732E-3</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>55.880270463099997</v>
       </c>
@@ -14176,7 +14174,7 @@
         <v>32.400602377799999</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>50.292243416799998</v>
       </c>
@@ -14205,7 +14203,7 @@
         <v>3.2400602377799999</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>45.563019075100001</v>
       </c>
@@ -14234,7 +14232,7 @@
         <v>3.0240060237800002</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>41.006717167600002</v>
       </c>
@@ -14263,7 +14261,7 @@
         <v>0.30240060237799998</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>36.906045450800001</v>
       </c>
@@ -14292,7 +14290,7 @@
         <v>3.0240060237800001E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>63.015440905799998</v>
       </c>
@@ -14321,7 +14319,7 @@
         <v>268.20302400600002</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>69.313896815199996</v>
       </c>
@@ -14350,7 +14348,7 @@
         <v>140.220302401</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>80.982507133699997</v>
       </c>
@@ -14379,7 +14377,7 @@
         <v>181.42203024</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>80.384256420300005</v>
       </c>
@@ -14408,7 +14406,7 @@
         <v>85.642203023999997</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>72.645830778299995</v>
       </c>
@@ -14437,7 +14435,7 @@
         <v>11.2642203024</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>65.981247700400004</v>
       </c>
@@ -14466,7 +14464,7 @@
         <v>6.52642203024</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>59.383122930399999</v>
       </c>
@@ -14495,7 +14493,7 @@
         <v>0.652642203024</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>53.444810637400003</v>
       </c>
@@ -14524,7 +14522,7 @@
         <v>6.5264220302400006E-2</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>48.1003295736</v>
       </c>
@@ -14553,7 +14551,7 @@
         <v>6.5264220302400002E-3</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>43.290296616299997</v>
       </c>
@@ -14582,7 +14580,7 @@
         <v>6.52642203024E-4</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>52.761266954600003</v>
       </c>
@@ -14611,7 +14609,7 @@
         <v>124.200065264</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>48.685140259199997</v>
       </c>
@@ -14640,7 +14638,7 @@
         <v>23.220006526399999</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>63.316626233299999</v>
       </c>
@@ -14669,7 +14667,7 @@
         <v>177.822000653</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>57.151633609900003</v>
       </c>
@@ -14698,7 +14696,7 @@
         <v>19.282230065299999</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>55.386470248899997</v>
       </c>
@@ -14727,7 +14725,7 @@
         <v>37.478223006500002</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>59.047823223999998</v>
       </c>
@@ -14756,7 +14754,7 @@
         <v>86.547822300700005</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>79.243040901599997</v>
       </c>
@@ -14785,7 +14783,7 @@
         <v>243.55478223</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>78.818736811500003</v>
       </c>
@@ -14814,7 +14812,7 @@
         <v>91.855478223000006</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>73.036863130300006</v>
       </c>
@@ -14843,7 +14841,7 @@
         <v>28.085547822300001</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>76.533176817300003</v>
       </c>
@@ -14872,7 +14870,7 @@
         <v>100.008554782</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>74.279859135600006</v>
       </c>
@@ -14901,7 +14899,7 @@
         <v>58.600855478200003</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>66.851873221999995</v>
       </c>
@@ -14930,7 +14928,7 @@
         <v>5.8600855478199998</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>60.166685899800001</v>
       </c>
@@ -14959,7 +14957,7 @@
         <v>0.58600855478199998</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>57.7500173098</v>
       </c>
@@ -14988,7 +14986,7 @@
         <v>32.458600855500002</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>51.975015578799997</v>
       </c>
@@ -15017,7 +15015,7 @@
         <v>3.2458600855499999</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>46.777514021000002</v>
       </c>
@@ -15046,7 +15044,7 @@
         <v>0.32458600855500003</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>43.899762618899999</v>
       </c>
@@ -15075,7 +15073,7 @@
         <v>16.232458600899999</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>39.509786357000003</v>
       </c>
@@ -15104,7 +15102,7 @@
         <v>1.6232458600899999</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>35.558807721299999</v>
       </c>
@@ -15133,7 +15131,7 @@
         <v>0.16232458600899999</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>32.002926949200003</v>
       </c>
@@ -15162,7 +15160,7 @@
         <v>1.6232458600900002E-2</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>31.202634254199999</v>
       </c>
@@ -15191,7 +15189,7 @@
         <v>21.601623245900001</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>32.282370828799998</v>
       </c>
@@ -15220,7 +15218,7 @@
         <v>39.960162324599999</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>32.054133745900003</v>
       </c>
@@ -15249,7 +15247,7 @@
         <v>30.996016232500001</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>28.848720371300001</v>
       </c>
@@ -15278,7 +15276,7 @@
         <v>3.0996016232499999</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>25.963848334200001</v>
       </c>
@@ -15307,7 +15305,7 @@
         <v>0.30996016232500001</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>23.3674635008</v>
       </c>
@@ -15336,7 +15334,7 @@
         <v>3.09960162325E-2</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>21.030717150699999</v>
       </c>
@@ -15365,7 +15363,7 @@
         <v>3.0996016232499998E-3</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>20.827645435600001</v>
       </c>
@@ -15394,7 +15392,7 @@
         <v>17.100309960200001</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>21.144880892100002</v>
       </c>
@@ -15423,7 +15421,7 @@
         <v>23.310030995999998</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>25.630392802900001</v>
       </c>
@@ -15452,7 +15450,7 @@
         <v>61.731003099600002</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>23.067353522600001</v>
       </c>
@@ -15481,7 +15479,7 @@
         <v>6.1731003099599997</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>25.5606181703</v>
       </c>
@@ -15510,7 +15508,7 @@
         <v>43.817310030999998</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>47.304556353300001</v>
       </c>
@@ -15539,7 +15537,7 @@
         <v>223.08173100299999</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>46.174100717999998</v>
       </c>
@@ -15568,7 +15566,7 @@
         <v>54.708173100300002</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>41.556690646200003</v>
       </c>
@@ -15597,7 +15595,7 @@
         <v>5.4708173100300002</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>37.401021581499997</v>
       </c>
@@ -15626,7 +15624,7 @@
         <v>0.54708173100299995</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>33.660919423400003</v>
       </c>
@@ -15655,7 +15653,7 @@
         <v>5.4708173100300003E-2</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>30.2948274811</v>
       </c>
@@ -15684,7 +15682,7 @@
         <v>5.4708173100300002E-3</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>27.265344732900001</v>
       </c>
@@ -15713,7 +15711,7 @@
         <v>5.4708173100300004E-4</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>24.5388102597</v>
       </c>
@@ -15742,7 +15740,7 @@
         <v>5.4708173100300002E-5</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>22.084929233699999</v>
       </c>
@@ -15771,7 +15769,7 @@
         <v>5.4708173100299999E-6</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>25.876436310300001</v>
       </c>
@@ -15800,7 +15798,7 @@
         <v>54.000000547100001</v>
       </c>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>28.3887926793</v>
       </c>
@@ -15829,7 +15827,7 @@
         <v>51.3000000547</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>49.549913411399999</v>
       </c>
@@ -15858,7 +15856,7 @@
         <v>221.130000005</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>44.594922070199999</v>
       </c>
@@ -15887,7 +15885,7 @@
         <v>22.113000000500001</v>
       </c>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>40.135429863200002</v>
       </c>
@@ -15916,7 +15914,7 @@
         <v>2.21130000005</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>40.321886876900003</v>
       </c>
@@ -15945,7 +15943,7 @@
         <v>38.021129999999999</v>
       </c>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>37.189698189200001</v>
       </c>
@@ -15974,7 +15972,7 @@
         <v>11.902113</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>38.470728370300002</v>
       </c>
@@ -16003,7 +16001,7 @@
         <v>46.190211300000001</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>41.223655533200002</v>
       </c>
@@ -16032,7 +16030,7 @@
         <v>64.019021129999999</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>49.701289979899997</v>
       </c>
@@ -16061,7 +16059,7 @@
         <v>119.801902113</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>44.731160981899997</v>
       </c>
@@ -16090,7 +16088,7 @@
         <v>11.9801902113</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>40.258044883700002</v>
       </c>
@@ -16119,7 +16117,7 @@
         <v>1.1980190211299999</v>
       </c>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>36.232240395399998</v>
       </c>
@@ -16148,7 +16146,7 @@
         <v>0.119801902113</v>
       </c>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>32.609016355800001</v>
       </c>
@@ -16177,7 +16175,7 @@
         <v>1.19801902113E-2</v>
       </c>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>38.348114720200002</v>
       </c>
@@ -16206,7 +16204,7 @@
         <v>81.001198019</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>39.013303248200003</v>
       </c>
@@ -16235,7 +16233,7 @@
         <v>48.6001198019</v>
       </c>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>42.311972923399999</v>
       </c>
@@ -16264,7 +16262,7 @@
         <v>69.660011980199997</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>38.980775631100002</v>
       </c>
@@ -16293,7 +16291,7 @@
         <v>15.066001198</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>43.082698067999999</v>
       </c>
@@ -16322,7 +16320,7 @@
         <v>73.506600119799998</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>39.674428261199999</v>
       </c>
@@ -16351,7 +16349,7 @@
         <v>15.450660012</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>64.206985435000007</v>
       </c>
@@ -16380,7 +16378,7 @@
         <v>258.04506600100001</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>67.086286891499995</v>
       </c>
@@ -16409,7 +16407,7 @@
         <v>109.5045066</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>63.977658202400001</v>
       </c>
@@ -16438,7 +16436,7 @@
         <v>43.35045066</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>59.279892382100002</v>
       </c>
@@ -16467,7 +16465,7 @@
         <v>19.635045066</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>53.351903143900003</v>
       </c>
@@ -16496,7 +16494,7 @@
         <v>1.9635045066000001</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>48.9167128295</v>
       </c>
@@ -16525,7 +16523,7 @@
         <v>8.2963504506600003</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>47.225041546600004</v>
       </c>
@@ -16554,7 +16552,7 @@
         <v>29.629635045099999</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>43.402537391899997</v>
       </c>
@@ -16583,7 +16581,7 @@
         <v>11.062963504500001</v>
       </c>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>51.062283652700003</v>
       </c>
@@ -16612,7 +16610,7 @@
         <v>109.10629634999999</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>54.056055287500001</v>
       </c>
@@ -16641,7 +16639,7 @@
         <v>83.810629634999998</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>48.650449758699999</v>
       </c>
@@ -16670,7 +16668,7 @@
         <v>8.3810629634999998</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>43.785404782800001</v>
       </c>
@@ -16699,7 +16697,7 @@
         <v>0.83810629635</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>39.406864304599999</v>
       </c>
@@ -16728,7 +16726,7 @@
         <v>8.3810629634999995E-2</v>
       </c>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>35.466177874099998</v>
       </c>
@@ -16757,7 +16755,7 @@
         <v>8.3810629635000002E-3</v>
       </c>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>31.919560086699999</v>
       </c>
@@ -16786,7 +16784,7 @@
         <v>8.3810629635000002E-4</v>
       </c>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>28.727604077999999</v>
       </c>
@@ -16815,7 +16813,7 @@
         <v>8.3810629634999993E-5</v>
       </c>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>28.854843670200001</v>
       </c>
@@ -16844,7 +16842,7 @@
         <v>27.000008381099999</v>
       </c>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>31.3693593032</v>
       </c>
@@ -16873,7 +16871,7 @@
         <v>51.300000838099997</v>
       </c>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>32.432423372899997</v>
       </c>
@@ -16902,7 +16900,7 @@
         <v>42.930000083800003</v>
       </c>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>33.089181035599999</v>
       </c>
@@ -16931,7 +16929,7 @@
         <v>39.393000008400001</v>
       </c>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>29.780262931999999</v>
       </c>
@@ -16960,7 +16958,7 @@
         <v>3.9393000008399999</v>
       </c>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>26.8022366388</v>
       </c>
@@ -16989,7 +16987,7 @@
         <v>0.39393000008399998</v>
       </c>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>39.122012974900002</v>
       </c>
@@ -17018,7 +17016,7 @@
         <v>135.03939299999999</v>
       </c>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>37.909811677500002</v>
       </c>
@@ -17047,7 +17045,7 @@
         <v>37.803939300000003</v>
       </c>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>35.918830509700001</v>
       </c>
@@ -17076,7 +17074,7 @@
         <v>19.980393930000002</v>
       </c>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>32.626947458700002</v>
       </c>
@@ -17105,7 +17103,7 @@
         <v>4.6980393930000002</v>
       </c>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>29.364252712900001</v>
       </c>
@@ -17134,7 +17132,7 @@
         <v>0.46980393929999997</v>
       </c>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>26.427827441600002</v>
       </c>
@@ -17163,7 +17161,7 @@
         <v>4.6980393930000003E-2</v>
       </c>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>26.7850446974</v>
       </c>
@@ -17192,7 +17190,7 @@
         <v>27.004698039400001</v>
       </c>
     </row>
-    <row r="289" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>26.806540227700001</v>
       </c>
@@ -17221,7 +17219,7 @@
         <v>27.0004698039</v>
       </c>
     </row>
-    <row r="290" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>24.125886204899999</v>
       </c>
@@ -17250,7 +17248,7 @@
         <v>2.7000469803899998</v>
       </c>
     </row>
-    <row r="291" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>23.813297584400001</v>
       </c>
@@ -17279,7 +17277,7 @@
         <v>19.170004698</v>
       </c>
     </row>
-    <row r="292" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>21.431967826000001</v>
       </c>
@@ -17308,7 +17306,7 @@
         <v>1.9170004698000001</v>
       </c>
     </row>
-    <row r="293" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>19.288771043400001</v>
       </c>
@@ -17337,7 +17335,7 @@
         <v>0.19170004698000001</v>
       </c>
     </row>
-    <row r="294" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>17.359893938999999</v>
       </c>
@@ -17366,7 +17364,7 @@
         <v>1.9170004697999999E-2</v>
       </c>
     </row>
-    <row r="295" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>15.6239045451</v>
       </c>
@@ -17395,7 +17393,7 @@
         <v>1.9170004698E-3</v>
       </c>
     </row>
-    <row r="296" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>14.061514090599999</v>
       </c>
@@ -17435,7 +17433,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17447,7 +17445,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>